<commit_message>
Added count down timer
</commit_message>
<xml_diff>
--- a/team-info.xlsx
+++ b/team-info.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21903"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="90" documentId="13_ncr:1_{8631949B-B9AB-41A9-9DC7-8B2C58C8D647}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{5CF8F68E-B41F-4D76-AC53-BCD41D7CDF34}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F87CEE7-ACC9-45E8-9AAF-B81DD7897F1D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,6 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -28,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="45">
   <si>
     <t>华语网辩报名信息</t>
   </si>
@@ -57,13 +56,13 @@
     <t>https://www.wjx.cn/jq/42413695.aspx</t>
   </si>
   <si>
-    <t>2019-07-05  00:01</t>
-  </si>
-  <si>
-    <t>2019-07-08  23:59</t>
-  </si>
-  <si>
-    <t>2019-07-09 08:00</t>
+    <t>2019-07-03  00:01</t>
+  </si>
+  <si>
+    <t>2019-07-05  10:00</t>
+  </si>
+  <si>
+    <t>https://www.wjx.cn/jq/42426112.aspx</t>
   </si>
   <si>
     <t>特别乐群队</t>
@@ -160,13 +159,16 @@
   </si>
   <si>
     <t>二等奖卡山谷，和女警看来你，家开的不能刷卡</t>
+  </si>
+  <si>
+    <t>2019-07-05 22:39</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -523,10 +525,10 @@
   <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17.25"/>
+  <sheetFormatPr defaultRowHeight="17.25" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="35.85546875" style="2" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="29" style="2" bestFit="1" customWidth="1"/>
@@ -538,12 +540,12 @@
     <col min="8" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="18">
+    <row r="2" spans="1:7" ht="18" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -566,7 +568,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>8</v>
       </c>
@@ -577,10 +579,10 @@
         <v>10</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>11</v>
+        <v>44</v>
       </c>
       <c r="F3" s="2" t="s">
         <v>12</v>
@@ -607,7 +609,7 @@
       <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17.25"/>
+  <sheetFormatPr defaultRowHeight="17.25" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="11.85546875" style="2" customWidth="1"/>
     <col min="2" max="2" width="11.140625" style="2" customWidth="1"/>
@@ -619,7 +621,7 @@
     <col min="8" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>14</v>
       </c>
@@ -633,7 +635,7 @@
       <c r="I1" s="4"/>
       <c r="J1" s="4"/>
     </row>
-    <row r="2" spans="1:10" ht="18">
+    <row r="2" spans="1:10" ht="18" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>15</v>
       </c>
@@ -654,7 +656,7 @@
       </c>
       <c r="G2" s="1"/>
     </row>
-    <row r="3" spans="1:10">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>21</v>
       </c>
@@ -674,7 +676,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="4" spans="1:10">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>27</v>
       </c>
@@ -694,7 +696,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="1:10">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>30</v>
       </c>
@@ -708,7 +710,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="6" spans="1:10">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>26</v>
       </c>
@@ -722,7 +724,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="7" spans="1:10">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>32</v>
       </c>
@@ -736,7 +738,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="8" spans="1:10">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>33</v>
       </c>
@@ -750,12 +752,12 @@
         <v>27</v>
       </c>
     </row>
-    <row r="9" spans="1:10">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="10" spans="1:10">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>35</v>
       </c>
@@ -773,7 +775,7 @@
       <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="17.25" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="12.85546875" style="7" customWidth="1"/>
     <col min="2" max="2" width="14.28515625" style="7" bestFit="1" customWidth="1"/>
@@ -781,7 +783,7 @@
     <col min="5" max="16384" width="9.140625" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="17.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="9" t="s">
         <v>36</v>
       </c>
@@ -789,7 +791,7 @@
       <c r="C1" s="9"/>
       <c r="D1" s="9"/>
     </row>
-    <row r="2" spans="1:6" ht="18">
+    <row r="2" spans="1:6" ht="18" x14ac:dyDescent="0.35">
       <c r="A2" s="8" t="s">
         <v>37</v>
       </c>
@@ -803,7 +805,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="3" spans="1:6" s="5" customFormat="1" ht="18">
+    <row r="3" spans="1:6" s="5" customFormat="1" ht="18" x14ac:dyDescent="0.35">
       <c r="A3" s="5" t="s">
         <v>41</v>
       </c>

</xml_diff>